<commit_message>
Update Levi‘s CMS Operation&Maintenance Request List_CHN.xlsx
</commit_message>
<xml_diff>
--- a/2019/总体管理/Levi‘s CMS Operation&Maintenance Request List_CHN.xlsx
+++ b/2019/总体管理/Levi‘s CMS Operation&Maintenance Request List_CHN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File Server\Tree Sapling\03 Levi's\gitCube-levisProject\2019\总体管理\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE6E4A8-008E-454B-B5D9-98C66624D354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9A4330-4E0E-4383-A397-A94EC80B5D54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="105">
   <si>
     <t>*</t>
   </si>
@@ -274,13 +274,6 @@
   </si>
   <si>
     <t>1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>王丽</t>
-  </si>
-  <si>
-    <t>王丽</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -421,6 +414,71 @@
   </si>
   <si>
     <t>任秋凤</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>【2019/11/25】
+为客户提取武汉店F2素材</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>运营执行</t>
+  </si>
+  <si>
+    <t>运营执行</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2019/11/25</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>门店长</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>辛红</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Kris</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2019/11/21</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>【2019/11/21】
+为客户提取香港店门头素材</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>【2019/11/22】
+已为客户提取香港店门头素材</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>【2019/11/26】
+已为客户提取香港店门头素材</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>154367
+114861
+154366</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>114878
+154127</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -910,7 +968,70 @@
     <cellStyle name="脱浦 [0.00]_laroux" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="脱浦_laroux" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="93">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3280,11 +3401,11 @@
   <dimension ref="A1:AD65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="F2" sqref="F2"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
+      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="12"/>
@@ -3370,7 +3491,7 @@
       </c>
       <c r="S2" s="15">
         <f>COUNTA(B6:B65)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T2" s="14" t="s">
         <v>1</v>
@@ -3415,7 +3536,7 @@
       <c r="S3" s="15">
         <f>COUNTIF(B:B,"确认
 完成")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T3" s="14" t="s">
         <v>2</v>
@@ -3532,7 +3653,7 @@
         <v>37</v>
       </c>
       <c r="U5" s="48" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V5" s="49"/>
       <c r="W5" s="19" t="s">
@@ -3562,13 +3683,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E6" s="39" t="s">
         <v>23</v>
@@ -3583,10 +3704,10 @@
         <v>25</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K6" s="40" t="s">
         <v>40</v>
@@ -3601,22 +3722,22 @@
         <v>60</v>
       </c>
       <c r="O6" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="P6" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q6" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="P6" s="44" t="s">
+      <c r="S6" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="42" t="s">
+      <c r="T6" s="43" t="s">
         <v>66</v>
-      </c>
-      <c r="R6" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="S6" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" s="43" t="s">
-        <v>68</v>
       </c>
       <c r="U6" s="50"/>
       <c r="V6" s="51"/>
@@ -3635,13 +3756,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>22</v>
@@ -3656,10 +3777,10 @@
         <v>24</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>40</v>
@@ -3674,22 +3795,22 @@
         <v>59</v>
       </c>
       <c r="O7" s="41" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="P7" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="42" t="s">
+      <c r="S7" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="R7" s="43" t="s">
+      <c r="T7" s="41" t="s">
         <v>79</v>
-      </c>
-      <c r="S7" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="T7" s="41" t="s">
-        <v>81</v>
       </c>
       <c r="U7" s="50"/>
       <c r="V7" s="51"/>
@@ -3718,31 +3839,31 @@
         <v>3</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F8" s="39" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H8" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="40" t="s">
         <v>83</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="40" t="s">
-        <v>85</v>
       </c>
       <c r="K8" s="40" t="s">
         <v>40</v>
@@ -3757,28 +3878,28 @@
         <v>59</v>
       </c>
       <c r="O8" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="P8" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q8" s="42" t="s">
         <v>86</v>
-      </c>
-      <c r="P8" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q8" s="42" t="s">
-        <v>88</v>
       </c>
       <c r="R8" s="40">
         <v>43760</v>
       </c>
       <c r="S8" s="41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="T8" s="43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="U8" s="50"/>
       <c r="V8" s="51"/>
       <c r="W8" s="16"/>
       <c r="X8" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Y8" s="21" t="s">
         <v>10</v>
@@ -3801,13 +3922,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>22</v>
@@ -3822,10 +3943,10 @@
         <v>24</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>40</v>
@@ -3840,28 +3961,28 @@
         <v>59</v>
       </c>
       <c r="O9" s="41" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="P9" s="44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q9" s="42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R9" s="43">
         <v>43770</v>
       </c>
       <c r="S9" s="41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="T9" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="U9" s="50"/>
       <c r="V9" s="51"/>
       <c r="W9" s="16"/>
       <c r="X9" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Y9" s="21" t="s">
         <v>14</v>
@@ -3878,35 +3999,73 @@
       <c r="AC9" s="23"/>
       <c r="AD9" s="23"/>
     </row>
-    <row r="10" spans="1:30" s="2" customFormat="1" ht="24">
-      <c r="A10" s="27">
+    <row r="10" spans="1:30" s="2" customFormat="1" ht="36">
+      <c r="A10" s="38">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="47"/>
+      <c r="B10" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="L10" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="P10" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q10" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="R10" s="43">
+        <v>43791</v>
+      </c>
+      <c r="S10" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="T10" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="U10" s="50"/>
+      <c r="V10" s="51"/>
       <c r="W10" s="16"/>
       <c r="X10" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Y10" s="21" t="s">
         <v>13</v>
@@ -3921,27 +4080,59 @@
       <c r="AC10" s="23"/>
       <c r="AD10" s="23"/>
     </row>
-    <row r="11" spans="1:30" s="2" customFormat="1">
+    <row r="11" spans="1:30" s="2" customFormat="1" ht="36">
       <c r="A11" s="27">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="32"/>
+      <c r="B11" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="L11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="P11" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q11" s="45" t="s">
+        <v>102</v>
+      </c>
       <c r="R11" s="31"/>
       <c r="S11" s="30"/>
       <c r="T11" s="31"/>
@@ -3951,7 +4142,9 @@
       <c r="X11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="Y11" s="21"/>
+      <c r="Y11" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="Z11" s="21" t="s">
         <v>49</v>
       </c>
@@ -5757,7 +5950,14 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="61">
-    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U58:V58"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="U53:V53"/>
+    <mergeCell ref="U54:V54"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="U56:V56"/>
+    <mergeCell ref="U57:V57"/>
     <mergeCell ref="U65:V65"/>
     <mergeCell ref="U59:V59"/>
     <mergeCell ref="U60:V60"/>
@@ -5765,14 +5965,6 @@
     <mergeCell ref="U62:V62"/>
     <mergeCell ref="U63:V63"/>
     <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U53:V53"/>
-    <mergeCell ref="U54:V54"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="U56:V56"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="U52:V52"/>
-    <mergeCell ref="U41:V41"/>
     <mergeCell ref="U42:V42"/>
     <mergeCell ref="U43:V43"/>
     <mergeCell ref="U44:V44"/>
@@ -5818,314 +6010,348 @@
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U14:V14"/>
     <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U7:V7"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="R27:T27 R30:T30 Q31:S31 F58:F63 G29:G30 F31:G31 G56:G63 F25:G28 F51:G55 D25:E31 D51:E63 D32:G50 Q28:T29 Q10:T25 Q9 C6:U6 O9:O25 C9:C29 D9:G24 C8:U8 D64:G65 C31:C65 P9:P65 H9:N65 Q51:T65 U10:U65">
-    <cfRule type="expression" dxfId="83" priority="424">
+  <conditionalFormatting sqref="R27:T27 R30:T30 Q31:S31 F58:F63 G29:G30 F31:G31 G56:G63 F25:G28 F51:G55 D25:E31 D51:E63 D32:G50 Q28:T29 Q10:T25 C6:N6 C9:C29 D9:G24 C8:U8 D64:G65 C31:C65 Q51:T65 U10:U65 P6:U6 P9:P65 O10:O25 H9:N65 Q9:Q11">
+    <cfRule type="expression" dxfId="92" priority="433">
       <formula>$B6="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="429">
+    <cfRule type="expression" dxfId="91" priority="438">
       <formula>$B6="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="430">
+    <cfRule type="expression" dxfId="90" priority="439">
       <formula>$B6="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q26:T26">
-    <cfRule type="expression" dxfId="80" priority="421">
+    <cfRule type="expression" dxfId="89" priority="430">
       <formula>$B26="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="422">
+    <cfRule type="expression" dxfId="88" priority="431">
       <formula>$B26="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="423">
+    <cfRule type="expression" dxfId="87" priority="432">
       <formula>$B26="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27">
-    <cfRule type="expression" dxfId="77" priority="403">
+    <cfRule type="expression" dxfId="86" priority="412">
       <formula>$B27="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="404">
+    <cfRule type="expression" dxfId="85" priority="413">
       <formula>$B27="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="405">
+    <cfRule type="expression" dxfId="84" priority="414">
       <formula>$B27="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="expression" dxfId="74" priority="400">
+    <cfRule type="expression" dxfId="83" priority="409">
       <formula>$B29="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="401">
+    <cfRule type="expression" dxfId="82" priority="410">
       <formula>$B29="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="402">
+    <cfRule type="expression" dxfId="81" priority="411">
       <formula>$B29="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30">
-    <cfRule type="expression" dxfId="71" priority="391">
+    <cfRule type="expression" dxfId="80" priority="400">
       <formula>$B30="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="392">
+    <cfRule type="expression" dxfId="79" priority="401">
       <formula>$B30="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="393">
+    <cfRule type="expression" dxfId="78" priority="402">
       <formula>$B30="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="expression" dxfId="68" priority="388">
+    <cfRule type="expression" dxfId="77" priority="397">
       <formula>$B30="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="389">
+    <cfRule type="expression" dxfId="76" priority="398">
       <formula>$B30="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="390">
+    <cfRule type="expression" dxfId="75" priority="399">
       <formula>$B30="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="65" priority="379">
+    <cfRule type="expression" dxfId="74" priority="388">
       <formula>$B30="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="380">
+    <cfRule type="expression" dxfId="73" priority="389">
       <formula>$B30="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="381">
+    <cfRule type="expression" dxfId="72" priority="390">
       <formula>$B30="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T31">
-    <cfRule type="expression" dxfId="62" priority="373">
+    <cfRule type="expression" dxfId="71" priority="382">
       <formula>$B31="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="374">
+    <cfRule type="expression" dxfId="70" priority="383">
       <formula>$B31="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="375">
+    <cfRule type="expression" dxfId="69" priority="384">
       <formula>$B31="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="expression" dxfId="59" priority="247">
+    <cfRule type="expression" dxfId="68" priority="256">
       <formula>$B56="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="248">
+    <cfRule type="expression" dxfId="67" priority="257">
       <formula>$B56="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="249">
+    <cfRule type="expression" dxfId="66" priority="258">
       <formula>$B56="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="expression" dxfId="56" priority="241">
+    <cfRule type="expression" dxfId="65" priority="250">
       <formula>$B57="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="242">
+    <cfRule type="expression" dxfId="64" priority="251">
       <formula>$B57="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="243">
+    <cfRule type="expression" dxfId="63" priority="252">
       <formula>$B57="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q32:S40">
-    <cfRule type="expression" dxfId="53" priority="139">
+    <cfRule type="expression" dxfId="62" priority="148">
       <formula>$B32="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="140">
+    <cfRule type="expression" dxfId="61" priority="149">
       <formula>$B32="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="141">
+    <cfRule type="expression" dxfId="60" priority="150">
       <formula>$B32="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T32:T40">
-    <cfRule type="expression" dxfId="50" priority="133">
+    <cfRule type="expression" dxfId="59" priority="142">
       <formula>$B32="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="134">
+    <cfRule type="expression" dxfId="58" priority="143">
       <formula>$B32="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="135">
+    <cfRule type="expression" dxfId="57" priority="144">
       <formula>$B32="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q41:S50">
-    <cfRule type="expression" dxfId="47" priority="127">
+    <cfRule type="expression" dxfId="56" priority="136">
       <formula>$B41="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="128">
+    <cfRule type="expression" dxfId="55" priority="137">
       <formula>$B41="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="129">
+    <cfRule type="expression" dxfId="54" priority="138">
       <formula>$B41="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T41:T50">
-    <cfRule type="expression" dxfId="44" priority="121">
+    <cfRule type="expression" dxfId="53" priority="130">
       <formula>$B41="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="122">
+    <cfRule type="expression" dxfId="52" priority="131">
       <formula>$B41="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="123">
+    <cfRule type="expression" dxfId="51" priority="132">
       <formula>$B41="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O51:O64 O27:O28">
-    <cfRule type="expression" dxfId="41" priority="55">
+    <cfRule type="expression" dxfId="50" priority="64">
       <formula>$B27="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="56">
+    <cfRule type="expression" dxfId="49" priority="65">
       <formula>$B27="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="57">
+    <cfRule type="expression" dxfId="48" priority="66">
       <formula>$B27="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O25:O27">
-    <cfRule type="expression" dxfId="38" priority="52">
+    <cfRule type="expression" dxfId="47" priority="61">
       <formula>$B25="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="53">
+    <cfRule type="expression" dxfId="46" priority="62">
       <formula>$B25="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="54">
+    <cfRule type="expression" dxfId="45" priority="63">
       <formula>$B25="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O29">
-    <cfRule type="expression" dxfId="35" priority="49">
+    <cfRule type="expression" dxfId="44" priority="58">
       <formula>$B29="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="50">
+    <cfRule type="expression" dxfId="43" priority="59">
       <formula>$B29="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="51">
+    <cfRule type="expression" dxfId="42" priority="60">
       <formula>$B29="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O30">
-    <cfRule type="expression" dxfId="32" priority="46">
+    <cfRule type="expression" dxfId="41" priority="55">
       <formula>$B30="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="47">
+    <cfRule type="expression" dxfId="40" priority="56">
       <formula>$B30="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="48">
+    <cfRule type="expression" dxfId="39" priority="57">
       <formula>$B30="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O31">
-    <cfRule type="expression" dxfId="29" priority="43">
+    <cfRule type="expression" dxfId="38" priority="52">
       <formula>$B31="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="44">
+    <cfRule type="expression" dxfId="37" priority="53">
       <formula>$B31="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="45">
+    <cfRule type="expression" dxfId="36" priority="54">
       <formula>$B31="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O65">
-    <cfRule type="expression" dxfId="26" priority="40">
+    <cfRule type="expression" dxfId="35" priority="49">
       <formula>$B65="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="41">
+    <cfRule type="expression" dxfId="34" priority="50">
       <formula>$B65="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="42">
+    <cfRule type="expression" dxfId="33" priority="51">
       <formula>$B65="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O32:O40">
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="32" priority="34">
       <formula>$B32="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="26">
+    <cfRule type="expression" dxfId="31" priority="35">
       <formula>$B32="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="27">
+    <cfRule type="expression" dxfId="30" priority="36">
       <formula>$B32="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O41:O50">
-    <cfRule type="expression" dxfId="20" priority="22">
+    <cfRule type="expression" dxfId="29" priority="31">
       <formula>$B41="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="23">
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>$B41="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="24">
+    <cfRule type="expression" dxfId="27" priority="33">
       <formula>$B41="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O24">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>$B24="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="25" priority="29">
       <formula>$B24="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="21">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>$B24="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9 T9">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="23" priority="22">
       <formula>$B9="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>$B9="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>$B9="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U9">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="20" priority="19">
       <formula>$B9="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>$B9="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="18" priority="21">
       <formula>$B9="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>$B9="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$B9="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>$B9="完了"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:T7">
-    <cfRule type="expression" dxfId="5" priority="4">
+  <conditionalFormatting sqref="C7:N7 P7:T7">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>$B7="暂停"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$B7="取消"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>$B7="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>$B7="暂停"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>$B7="取消"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>$B7="完了"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>$B7="暂停"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$B7="取消"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>$B7="完了"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>$B6="暂停"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>$B6="取消"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>$B6="完了"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$B7="暂停"</formula>
+      <formula>$B9="暂停"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$B7="取消"</formula>
+      <formula>$B9="取消"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$B7="完了"</formula>
+      <formula>$B9="完了"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>